<commit_message>
Update to the Excel document.
</commit_message>
<xml_diff>
--- a/eBayProject/src/test/resources/testdata/Test_scenarios.xlsx
+++ b/eBayProject/src/test/resources/testdata/Test_scenarios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\git\eBayProject\eBayProject\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Test scenario</t>
   </si>
@@ -60,21 +60,12 @@
     <t>For an unlogged user, navigate to the Cart page from the Main page, and click on the 'Start shopping' link, and verify that it brings user to the Main page again</t>
   </si>
   <si>
-    <t>For an unlogged user, search for any item via the Search box, add one item to the cart, then navigate to the cart and verify that it displays the correct item and price</t>
-  </si>
-  <si>
     <t>For an unlogged user, navigate to the Cart page from the Main page and verify if the title and URL are correct</t>
   </si>
   <si>
     <t>TC004</t>
   </si>
   <si>
-    <t>Designed by:</t>
-  </si>
-  <si>
-    <t>Last updated by:</t>
-  </si>
-  <si>
     <t>Last update date:</t>
   </si>
   <si>
@@ -96,9 +87,6 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>Testing covers a few basic scenarios on the Cart page of the eBay page.</t>
-  </si>
-  <si>
     <t>Aleksandra M</t>
   </si>
   <si>
@@ -111,9 +99,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>PASSED/FAILED:</t>
-  </si>
-  <si>
     <t>PASSED</t>
   </si>
   <si>
@@ -121,13 +106,40 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>For an unlogged user, search for any item via the Search box, add one item to the cart, then navigate to the cart and verify that it displays the correct price for them item, and then remove the item from the cart</t>
+  </si>
+  <si>
+    <t>Testing covers a few basic test cases on the Cart page of the eBay page.</t>
+  </si>
+  <si>
+    <t>Test designed by:</t>
+  </si>
+  <si>
+    <t>Test approved by:</t>
+  </si>
+  <si>
+    <t>Document last updated by:</t>
+  </si>
+  <si>
+    <t>Last status (PASSED/FAILED):</t>
+  </si>
+  <si>
+    <t>Comments on the last test run:</t>
+  </si>
+  <si>
+    <t>URL address of a website tested:</t>
+  </si>
+  <si>
+    <t>https://www.ebay.com/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +152,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -184,10 +205,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -222,8 +244,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -502,16 +528,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C15"/>
+  <dimension ref="B1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="28" style="7" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" style="7" customWidth="1"/>
     <col min="3" max="3" width="38.28515625" style="7" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="7"/>
   </cols>
@@ -519,109 +543,120 @@
     <row r="1" spans="2:3" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>18</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>22</v>
+        <v>34</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="9" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
+      <c r="B6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>24</v>
-      </c>
+      <c r="B7" s="8"/>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="10">
+      <c r="C9" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="10">
         <v>43466</v>
       </c>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="8"/>
-    </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>24</v>
-      </c>
+      <c r="B11" s="8"/>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="10">
-        <v>43467</v>
+        <v>14</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>29</v>
+        <v>13</v>
+      </c>
+      <c r="C14" s="10">
+        <v>43467</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -629,9 +664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -669,7 +702,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="45" x14ac:dyDescent="0.25">
@@ -692,14 +725,14 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added a new test case to a CartPageTest class, fixed a bug in a CartPage class, and updated relevant classes.
</commit_message>
<xml_diff>
--- a/eBayProject/src/test/resources/testdata/Test_scenarios.xlsx
+++ b/eBayProject/src/test/resources/testdata/Test_scenarios.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\git\eBayProject\eBayProject\src\test\resources\testdata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9540" windowHeight="2760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="4350"/>
   </bookViews>
   <sheets>
     <sheet name="Test_details" sheetId="1" r:id="rId1"/>
     <sheet name="Test_scenarios_Cart_page" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A4:G15"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Test scenario</t>
   </si>
@@ -133,6 +129,12 @@
   </si>
   <si>
     <t>https://www.ebay.com/</t>
+  </si>
+  <si>
+    <t>TC005</t>
+  </si>
+  <si>
+    <t>For an unlogged user, open Cart page on its own, click on the 'Send Us Your Comments' link, verify if it brings user to the correct page, and fill in a feedback form</t>
   </si>
 </sst>
 </file>
@@ -528,9 +530,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -643,7 +645,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
         <v>33</v>
       </c>
@@ -662,9 +664,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:E20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -725,19 +729,25 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="D7" s="2"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>

</xml_diff>

<commit_message>
Updated the test data file.
</commit_message>
<xml_diff>
--- a/eBayProject/src/test/resources/testdata/Test_scenarios.xlsx
+++ b/eBayProject/src/test/resources/testdata/Test_scenarios.xlsx
@@ -4,14 +4,15 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12495" windowHeight="4350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="3720" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test_details" sheetId="1" r:id="rId1"/>
-    <sheet name="Test_scenarios_Cart_page" sheetId="2" r:id="rId2"/>
+    <sheet name="Test_Scenarios_Search_page" sheetId="3" r:id="rId2"/>
+    <sheet name="Test_scenarios_Cart_page" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A4:G15"/>
+  <oleSize ref="A1:F7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Test scenario</t>
   </si>
@@ -135,6 +136,15 @@
   </si>
   <si>
     <t>For an unlogged user, open Cart page on its own, click on the 'Send Us Your Comments' link, verify if it brings user to the correct page, and fill in a feedback form</t>
+  </si>
+  <si>
+    <t>Verify if the left bar displaying feaures (Color, Shape, Price, etc.) works correctly</t>
+  </si>
+  <si>
+    <t>From Main page, navigate to the Search page by filling in the Search input field and clicking Search button</t>
+  </si>
+  <si>
+    <t>On Search page, select a Shape value, e.g. "Round"</t>
   </si>
 </sst>
 </file>
@@ -532,7 +542,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -664,10 +674,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="1.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6"/>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated the Chrome drivers to version 78.0.3904.105.
</commit_message>
<xml_diff>
--- a/eBayProject/src/test/resources/testdata/Test_scenarios.xlsx
+++ b/eBayProject/src/test/resources/testdata/Test_scenarios.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aleks\git\eBayProject\eBayProject\src\test\resources\testdata\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="3720" firstSheet="1" activeTab="1"/>
   </bookViews>
@@ -10,9 +15,9 @@
     <sheet name="Test_details" sheetId="1" r:id="rId1"/>
     <sheet name="Test_Scenarios_Search_page" sheetId="3" r:id="rId2"/>
     <sheet name="Test_scenarios_Cart_page" sheetId="2" r:id="rId3"/>
+    <sheet name="Test_scenarios_Cart_page #TC001" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:F7"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="56">
   <si>
     <t>Test scenario</t>
   </si>
@@ -51,18 +56,12 @@
     <t>TC002</t>
   </si>
   <si>
-    <t>TC003</t>
-  </si>
-  <si>
     <t>For an unlogged user, navigate to the Cart page from the Main page, and click on the 'Start shopping' link, and verify that it brings user to the Main page again</t>
   </si>
   <si>
     <t>For an unlogged user, navigate to the Cart page from the Main page and verify if the title and URL are correct</t>
   </si>
   <si>
-    <t>TC004</t>
-  </si>
-  <si>
     <t>Last update date:</t>
   </si>
   <si>
@@ -132,9 +131,6 @@
     <t>https://www.ebay.com/</t>
   </si>
   <si>
-    <t>TC005</t>
-  </si>
-  <si>
     <t>For an unlogged user, open Cart page on its own, click on the 'Send Us Your Comments' link, verify if it brings user to the correct page, and fill in a feedback form</t>
   </si>
   <si>
@@ -145,6 +141,61 @@
   </si>
   <si>
     <t>On Search page, select a Shape value, e.g. "Round"</t>
+  </si>
+  <si>
+    <t>#TC001</t>
+  </si>
+  <si>
+    <t>#TC002</t>
+  </si>
+  <si>
+    <t>#TC003</t>
+  </si>
+  <si>
+    <t>#TC004</t>
+  </si>
+  <si>
+    <t>#TC005</t>
+  </si>
+  <si>
+    <t>#TS001</t>
+  </si>
+  <si>
+    <t>#TC0001</t>
+  </si>
+  <si>
+    <t>Steps:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User is not logged in. </t>
+  </si>
+  <si>
+    <t>Prerequisites</t>
+  </si>
+  <si>
+    <t>1. In the browser, open the Main page (http://www.ebay.com/)</t>
+  </si>
+  <si>
+    <t>2. In the header, click on the Cart page.</t>
+  </si>
+  <si>
+    <t>Expected result:</t>
+  </si>
+  <si>
+    <t>Actual result:</t>
+  </si>
+  <si>
+    <t>3. When the Cart oage loads, verify the title of the page and the URL.</t>
+  </si>
+  <si>
+    <t>The URL should be "https://cart.payments.ebay.com/".
+The title should be "Shopping cart".</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Test case - short description</t>
   </si>
 </sst>
 </file>
@@ -179,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +240,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,7 +278,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -258,6 +315,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -540,7 +600,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="B1:C16"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
@@ -555,42 +615,42 @@
     <row r="1" spans="2:3" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -598,23 +658,23 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" s="10">
         <v>43466</v>
@@ -625,23 +685,23 @@
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="10">
         <v>43467</v>
@@ -649,18 +709,18 @@
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -690,11 +750,8 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
@@ -708,18 +765,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:5" s="1" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -729,7 +786,7 @@
         <v>8</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -763,10 +820,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="B1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,28 +848,28 @@
         <v>2</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
-        <v>5</v>
+        <v>43</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="5"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>7</v>
@@ -822,30 +879,30 @@
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
       <c r="D5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>9</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
       <c r="C6" s="6"/>
       <c r="D6" s="5" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="75" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="5" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -901,4 +958,95 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="65.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="13"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="13"/>
+      <c r="C8" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="13"/>
+      <c r="C9" s="6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the excel and images Small changes in the code
</commit_message>
<xml_diff>
--- a/eBayProject/src/test/resources/testdata/Test_scenarios.xlsx
+++ b/eBayProject/src/test/resources/testdata/Test_scenarios.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="3720" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="3720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test_details" sheetId="1" r:id="rId1"/>
@@ -230,7 +230,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -246,6 +246,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,9 +295,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -318,6 +321,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -602,124 +608,124 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:C16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="38.28515625" style="7" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="2.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="38.28515625" style="6" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
+      <c r="B7" s="7"/>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="9">
         <v>43466</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="8"/>
+      <c r="B11" s="7"/>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="13" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <v>43467</v>
       </c>
     </row>
     <row r="15" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B16" s="11" t="s">
+      <c r="B16" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>21</v>
       </c>
     </row>
@@ -736,8 +742,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,66 +758,66 @@
   <sheetData>
     <row r="1" spans="2:5" ht="8.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="13" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="5"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -822,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -838,70 +844,70 @@
   <sheetData>
     <row r="1" spans="2:5" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="13" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="3" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="5" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="5" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>25</v>
       </c>
     </row>
@@ -978,70 +984,70 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="13"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="6" t="s">
+      <c r="B7" s="12"/>
+      <c r="C7" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="13"/>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>54</v>
       </c>
     </row>

</xml_diff>